<commit_message>
reads no. of rows and cols worksheet's data read thru for loop.
</commit_message>
<xml_diff>
--- a/wrksht.xlsx
+++ b/wrksht.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="First" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -421,7 +421,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>